<commit_message>
Updated tranformed data sets based on removal of extreme outlier
Update transformations based on removal on one instance that was an extreme outlier
</commit_message>
<xml_diff>
--- a/outputs/demos_22-0620.xlsx
+++ b/outputs/demos_22-0620.xlsx
@@ -8,19 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarr\Documents\GitHub\predictive-modeling\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81713E26-F2B0-4F7D-84DE-92C84213925E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D110DAE2-5A45-4EC3-BB48-36B872C7E854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demos_22-0620" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="131">
   <si>
     <t>metric</t>
   </si>
@@ -407,6 +419,12 @@
   </si>
   <si>
     <t>Filtered Out</t>
+  </si>
+  <si>
+    <t>Range Low Diff</t>
+  </si>
+  <si>
+    <t>Range High Diff</t>
   </si>
 </sst>
 </file>
@@ -549,7 +567,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +771,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -914,7 +938,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -935,6 +959,9 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -980,7 +1007,57 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1292,11 +1369,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AO1" sqref="AO1"/>
+      <selection pane="bottomRight" activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,7 +1522,7 @@
       <c r="E2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="12" t="s">
         <v>46</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -1463,7 +1540,7 @@
       <c r="K2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="12" t="s">
         <v>52</v>
       </c>
       <c r="M2" s="3" t="s">
@@ -1499,7 +1576,7 @@
       <c r="W2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="12" t="s">
         <v>64</v>
       </c>
       <c r="Y2" s="5" t="s">
@@ -5023,27 +5100,731 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>129</v>
+      </c>
+      <c r="B32">
+        <f>B30-B12</f>
+        <v>1.4140000000000001</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:AP32" si="0">C30-C12</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>11.1</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="0"/>
+        <v>2.621</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="0"/>
+        <v>0.33899999999999997</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="0"/>
+        <v>3.234</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="0"/>
+        <v>2.8999999999999915E-2</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="0"/>
+        <v>0.11699999999999999</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <f t="shared" si="0"/>
+        <v>0.6180000000000001</v>
+      </c>
+      <c r="AC32">
+        <f t="shared" si="0"/>
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="AD32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AG32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" si="0"/>
+        <v>0.91699999999999982</v>
+      </c>
+      <c r="AO32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33">
+        <f>B13-B31</f>
+        <v>0.1800000000000006</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:AP33" si="1">C13-C31</f>
+        <v>2.274</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="1"/>
+        <v>2.6540000000000004</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>0.48199999999999932</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>0.7799999999999998</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="1"/>
+        <v>0.15100000000000002</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="1"/>
+        <v>0.14599999999999991</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="1"/>
+        <v>0.12800000000000011</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="1"/>
+        <v>132</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AB33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC33">
+        <f t="shared" si="1"/>
+        <v>0.629</v>
+      </c>
+      <c r="AD33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AE33">
+        <f t="shared" si="1"/>
+        <v>22.473999999999997</v>
+      </c>
+      <c r="AF33">
+        <f t="shared" si="1"/>
+        <v>8.6059999999999999</v>
+      </c>
+      <c r="AG33">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="AI33">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="AJ33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AK33">
+        <f t="shared" si="1"/>
+        <v>4.8840000000000003</v>
+      </c>
+      <c r="AL33">
+        <f t="shared" si="1"/>
+        <v>1.3330000000000002</v>
+      </c>
+      <c r="AM33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AN33">
+        <f t="shared" si="1"/>
+        <v>3.0289999999999999</v>
+      </c>
+      <c r="AO33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>127</v>
       </c>
+      <c r="B34">
+        <f>B32/B9</f>
+        <v>2.6233766233766236</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:AP34" si="2">C32/C9</f>
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>1.2381483547127718</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="2"/>
+        <v>3.3602564102564103</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>0.57849829351535831</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="2"/>
+        <v>3.5267175572519083</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="2"/>
+        <v>0.9666666666666639</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="2"/>
+        <v>1.21875</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <f t="shared" si="2"/>
+        <v>2.7837837837837842</v>
+      </c>
+      <c r="AC34">
+        <f t="shared" si="2"/>
+        <v>5.2356687898089165</v>
+      </c>
+      <c r="AD34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AF34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AH34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AM34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AN34">
+        <f t="shared" si="2"/>
+        <v>0.75722543352601135</v>
+      </c>
+      <c r="AO34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>125</v>
       </c>
+      <c r="B35">
+        <f>B33/B9</f>
+        <v>0.3339517625231922</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:AP35" si="3">C33/C9</f>
+        <v>2.8460575719649559</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="3"/>
+        <v>4.8043925875085787</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>11.07011070110701</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="3"/>
+        <v>11.391375101708705</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>8.0402010050251249</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="3"/>
+        <v>3.6596523330283626</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>8.7134802665299844</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="3"/>
+        <v>2.759381898454746</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="3"/>
+        <v>10.119595216191351</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="3"/>
+        <v>3.4025641025641029</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="3"/>
+        <v>0.82252559726962349</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="3"/>
+        <v>0.98984771573604036</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="3"/>
+        <v>5.2677787532923617</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="3"/>
+        <v>3.212765957446809</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="3"/>
+        <v>4.8666666666666636</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="3"/>
+        <v>18.518518518518519</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="3"/>
+        <v>6.1162079510703364</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="3"/>
+        <v>9.2592592592592595</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333346</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="3"/>
+        <v>25.109377972227509</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="3"/>
+        <v>5.2356020942408374</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="3"/>
+        <v>14.492753623188406</v>
+      </c>
+      <c r="AB35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC35">
+        <f t="shared" si="3"/>
+        <v>4.0063694267515926</v>
+      </c>
+      <c r="AD35">
+        <f t="shared" si="3"/>
+        <v>6.1349693251533743</v>
+      </c>
+      <c r="AE35">
+        <f t="shared" si="3"/>
+        <v>1.8687843006818556</v>
+      </c>
+      <c r="AF35">
+        <f t="shared" si="3"/>
+        <v>3.987951807228916</v>
+      </c>
+      <c r="AG35">
+        <f t="shared" si="3"/>
+        <v>11.308562197092083</v>
+      </c>
+      <c r="AH35">
+        <f t="shared" si="3"/>
+        <v>4.6604527296937412</v>
+      </c>
+      <c r="AI35">
+        <f t="shared" si="3"/>
+        <v>4.2319085907744389</v>
+      </c>
+      <c r="AJ35">
+        <f t="shared" si="3"/>
+        <v>2.3510971786833856</v>
+      </c>
+      <c r="AK35">
+        <f t="shared" si="3"/>
+        <v>5.1792152704135743</v>
+      </c>
+      <c r="AL35">
+        <f t="shared" si="3"/>
+        <v>2.0828125000000002</v>
+      </c>
+      <c r="AM35">
+        <f t="shared" si="3"/>
+        <v>3.5971223021582732</v>
+      </c>
+      <c r="AN35">
+        <f t="shared" si="3"/>
+        <v>2.5012386457473159</v>
+      </c>
+      <c r="AO35">
+        <f t="shared" si="3"/>
+        <v>8.6206896551724146</v>
+      </c>
+      <c r="AP35">
+        <f t="shared" si="3"/>
+        <v>8.3702609551944853</v>
+      </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="F36">
+        <f>F9*10</f>
+        <v>24.580000000000002</v>
+      </c>
+      <c r="L36">
+        <f>L9*10</f>
+        <v>32.61</v>
+      </c>
+      <c r="X36">
+        <f>X9*10</f>
+        <v>52.569999999999993</v>
+      </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>128</v>
       </c>
+      <c r="F37">
+        <f>ROUNDUP(F36+F31,0)</f>
+        <v>33</v>
+      </c>
+      <c r="L37">
+        <f>ROUNDUP(L36+L31,0)</f>
+        <v>44</v>
+      </c>
+      <c r="X37">
+        <f>ROUNDUP(X36+X31,0)</f>
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B35:AP35">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>B35&gt;5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:AP35">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>B35&gt;10</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>B35&gt;15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>